<commit_message>
Major update from Home
</commit_message>
<xml_diff>
--- a/Semester_4/BIO212/Bee_data/bee_data_from audio.xlsx
+++ b/Semester_4/BIO212/Bee_data/bee_data_from audio.xlsx
@@ -9,12 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="16">
   <si>
     <t>Magenta</t>
   </si>
@@ -68,6 +73,12 @@
   </si>
   <si>
     <t>Time Spent searching</t>
+  </si>
+  <si>
+    <t>Purple and White</t>
+  </si>
+  <si>
+    <t>Dark Purple</t>
   </si>
 </sst>
 </file>
@@ -391,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +450,7 @@
         <v>28.36</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D6" si="0">C3-B3</f>
         <v>13.266999999999999</v>
       </c>
       <c r="E3" s="1">
@@ -462,7 +473,7 @@
         <v>11.291</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <f t="shared" ref="E4:E6" si="1">B4-C3</f>
         <v>1.0100000000000016</v>
       </c>
     </row>
@@ -793,7 +804,7 @@
         <v>21.155000000000001</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
         <v>0.81500000000000128</v>
       </c>
       <c r="E3" s="1">
@@ -816,7 +827,7 @@
         <v>5.57</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <f t="shared" ref="E4:E13" si="1">B4-C3</f>
         <v>0.61499999999999844</v>
       </c>
     </row>
@@ -1204,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,4 +2439,2464 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.1549999999999998</v>
+      </c>
+      <c r="C2">
+        <v>2.5169999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2-B2</f>
+        <v>0.3620000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4.968</v>
+      </c>
+      <c r="C3">
+        <v>13.109</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <v>8.141</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3-C2</f>
+        <v>2.4510000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>13.833</v>
+      </c>
+      <c r="C4">
+        <v>14.446</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61299999999999955</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <v>0.7240000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>16.039000000000001</v>
+      </c>
+      <c r="C5">
+        <v>26.001000000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9619999999999997</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5930000000000017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>26.614000000000001</v>
+      </c>
+      <c r="C6">
+        <v>40.631</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.016999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.61299999999999955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>41.308999999999997</v>
+      </c>
+      <c r="C7">
+        <v>55.07</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>13.761000000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67799999999999727</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>57.79</v>
+      </c>
+      <c r="C8">
+        <v>58.704000000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.91400000000000148</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7199999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>59.807000000000002</v>
+      </c>
+      <c r="C9">
+        <v>60.54</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73299999999999699</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1030000000000015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>64.81</v>
+      </c>
+      <c r="C10">
+        <v>71.05</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2399999999999949</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>4.2700000000000031</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>78.838999999999999</v>
+      </c>
+      <c r="C11">
+        <v>81.781000000000006</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9420000000000073</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>7.7890000000000015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>82.091999999999999</v>
+      </c>
+      <c r="C12">
+        <v>85.394999999999996</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3029999999999973</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31099999999999284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>88.154399999999995</v>
+      </c>
+      <c r="C13">
+        <v>98.611999999999995</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>10.457599999999999</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7593999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>99.328000000000003</v>
+      </c>
+      <c r="C14">
+        <v>100.52200000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1940000000000026</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.71600000000000819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>100.875</v>
+      </c>
+      <c r="C15">
+        <v>123.80200000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>22.927000000000007</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.35299999999999443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>125.33799999999999</v>
+      </c>
+      <c r="C16">
+        <v>128.459</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1210000000000093</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5359999999999872</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>128.91800000000001</v>
+      </c>
+      <c r="C17">
+        <v>171.66900000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>42.751000000000005</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45900000000000318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C2">
+        <v>5.694</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2-B2</f>
+        <v>5.6349999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.0880000000000001</v>
+      </c>
+      <c r="C3">
+        <v>7.476</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3-C2</f>
+        <v>0.39400000000000013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>9.1</v>
+      </c>
+      <c r="C4">
+        <v>11.611000000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.511000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <v>1.6239999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>11.983000000000001</v>
+      </c>
+      <c r="C5">
+        <v>21.567</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5839999999999996</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37199999999999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>22.53</v>
+      </c>
+      <c r="C6">
+        <v>37.204999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.674999999999997</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.96300000000000097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>39.960999999999999</v>
+      </c>
+      <c r="C7">
+        <v>40.784999999999997</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.82399999999999807</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7560000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>42.853000000000002</v>
+      </c>
+      <c r="C8">
+        <v>43.475999999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.62299999999999756</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0680000000000049</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="C2">
+        <v>1.702</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2-B2</f>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>5.8360000000000003</v>
+      </c>
+      <c r="C3">
+        <v>26.0153</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <v>20.179299999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3-C2</f>
+        <v>4.1340000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>26.315999999999999</v>
+      </c>
+      <c r="C4">
+        <v>33.612000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2960000000000029</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <v>0.30069999999999908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>34.06</v>
+      </c>
+      <c r="C5">
+        <v>40.668999999999997</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6089999999999947</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4480000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>42.104999999999997</v>
+      </c>
+      <c r="C6">
+        <v>43.756999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.652000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4359999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>44.191000000000003</v>
+      </c>
+      <c r="C7">
+        <v>45.67</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4789999999999992</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4340000000000046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>47.006999999999998</v>
+      </c>
+      <c r="C8">
+        <v>70.447000000000003</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>23.440000000000005</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3369999999999962</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="C2">
+        <v>14.96</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2-B2</f>
+        <v>14.018000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>15.948</v>
+      </c>
+      <c r="C3">
+        <v>16.919</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <v>0.97100000000000009</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3-C2</f>
+        <v>0.98799999999999955</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>18.574999999999999</v>
+      </c>
+      <c r="C4">
+        <v>35.779000000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>17.204000000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <v>1.6559999999999988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>36.392000000000003</v>
+      </c>
+      <c r="C5">
+        <v>37.54</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1479999999999961</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.61299999999999955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>37.86</v>
+      </c>
+      <c r="C6">
+        <v>58.426000000000002</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>20.566000000000003</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32000000000000028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>59.000999999999998</v>
+      </c>
+      <c r="C7">
+        <v>77.084999999999994</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>18.083999999999996</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.57499999999999574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>77.525999999999996</v>
+      </c>
+      <c r="C8">
+        <v>88.334000000000003</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>10.808000000000007</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4410000000000025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>91.238</v>
+      </c>
+      <c r="C9">
+        <v>98.962500000000006</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7245000000000061</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9039999999999964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>99.983000000000004</v>
+      </c>
+      <c r="C10">
+        <v>101.021</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0379999999999967</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0204999999999984</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>103.44499999999999</v>
+      </c>
+      <c r="C11">
+        <v>109.42700000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9820000000000135</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4239999999999924</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>110.01</v>
+      </c>
+      <c r="C12">
+        <v>117.462</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4519999999999982</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.58299999999999841</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>118.0488</v>
+      </c>
+      <c r="C13">
+        <v>136.94800000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>18.899200000000008</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.58679999999999666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>137.22999999999999</v>
+      </c>
+      <c r="C14">
+        <v>150.43199999999999</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>13.201999999999998</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28199999999998226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>150.821</v>
+      </c>
+      <c r="C15">
+        <v>151.59</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76900000000000546</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>151.91800000000001</v>
+      </c>
+      <c r="C16">
+        <v>155.13200000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2139999999999986</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32800000000000296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>155.58000000000001</v>
+      </c>
+      <c r="C17">
+        <v>188.066</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>32.48599999999999</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4480000000000075</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>188.46799999999999</v>
+      </c>
+      <c r="C18">
+        <v>192.57</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1020000000000039</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40199999999998681</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>194.08199999999999</v>
+      </c>
+      <c r="C19">
+        <v>194.54900000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46700000000001296</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5120000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>194.54900000000001</v>
+      </c>
+      <c r="C20">
+        <v>196.21199999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6629999999999825</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>197.6429</v>
+      </c>
+      <c r="C21">
+        <v>219.77799999999999</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>22.135099999999994</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4309000000000083</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>220.02799999999999</v>
+      </c>
+      <c r="C22">
+        <v>234.99199999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>14.963999999999999</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>236.35</v>
+      </c>
+      <c r="C23">
+        <v>252.63800000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>16.288000000000011</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3580000000000041</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>253.054</v>
+      </c>
+      <c r="C24">
+        <v>253.74199999999999</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68799999999998818</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.41599999999999682</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>254.61500000000001</v>
+      </c>
+      <c r="C25">
+        <v>269.33699999999999</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>14.72199999999998</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.87300000000001887</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>270.22500000000002</v>
+      </c>
+      <c r="C26">
+        <v>271.76499999999999</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5399999999999636</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88800000000003365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>271.76499999999999</v>
+      </c>
+      <c r="C27">
+        <v>272.32499999999999</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000227</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>273.08999999999997</v>
+      </c>
+      <c r="C28">
+        <v>284.80500000000001</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>11.715000000000032</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76499999999998636</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>285.19099999999997</v>
+      </c>
+      <c r="C29">
+        <v>286.3</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1090000000000373</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38599999999996726</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>289.34300000000002</v>
+      </c>
+      <c r="C30">
+        <v>308.13099999999997</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>18.787999999999954</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0430000000000064</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>309.12</v>
+      </c>
+      <c r="C31">
+        <v>309.99799999999999</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8779999999999859</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
+        <v>0.98900000000003274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>310.52199999999999</v>
+      </c>
+      <c r="C32">
+        <v>315</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4780000000000086</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="1"/>
+        <v>0.52400000000000091</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>316.79700000000003</v>
+      </c>
+      <c r="C33">
+        <v>317.89100000000002</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0939999999999941</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7970000000000255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>318.26799999999997</v>
+      </c>
+      <c r="C34">
+        <v>327.57499999999999</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3070000000000164</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37699999999995271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>327.95400000000001</v>
+      </c>
+      <c r="C35">
+        <v>335.34300000000002</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>7.38900000000001</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="1"/>
+        <v>0.3790000000000191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>335.63299999999998</v>
+      </c>
+      <c r="C36">
+        <v>347.935</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>12.302000000000021</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28999999999996362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>348.10599999999999</v>
+      </c>
+      <c r="C37">
+        <v>350.57299999999998</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4669999999999845</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17099999999999227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>350.96100000000001</v>
+      </c>
+      <c r="C38">
+        <v>352.65199999999999</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6909999999999741</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38800000000003365</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.24</v>
+      </c>
+      <c r="C2">
+        <v>18.896999999999998</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2-B2</f>
+        <v>15.656999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>21.422999999999998</v>
+      </c>
+      <c r="C3">
+        <v>48.594000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D64" si="0">C3-B3</f>
+        <v>27.171000000000003</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3-C2</f>
+        <v>2.5259999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>50.267000000000003</v>
+      </c>
+      <c r="C4">
+        <v>52.256</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9889999999999972</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E64" si="1">B4-C3</f>
+        <v>1.6730000000000018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>